<commit_message>
invert binary tree and dynamic programming
</commit_message>
<xml_diff>
--- a/algoexpert/Algorithms_solved.xlsx
+++ b/algoexpert/Algorithms_solved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shehryarbajwa/algorithms-challenges/algoexpert/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D05A9F8-5C1D-E44B-8BD1-FC23699AA991}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB91804C-D589-664B-9D80-BF1334826027}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="60" windowWidth="28040" windowHeight="15900" xr2:uid="{5B13E3C5-C034-6249-A945-F210C27A470A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
   <si>
     <t>Problem</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>PreOrder, InOrder and PostOrder</t>
+  </si>
+  <si>
+    <t>Pre-order means append to array first, then traverse left, then right. Post-order append last, in Order means append in the middle</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to traverse through the tree, </t>
   </si>
 </sst>
 </file>
@@ -643,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692D23BF-E5BD-4744-931C-2F3DDC23964E}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,6 +1225,10 @@
       <c r="E21" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -1232,6 +1245,32 @@
       </c>
       <c r="E22" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>